<commit_message>
Refactoring code + Test cases update + improvements
</commit_message>
<xml_diff>
--- a/Test cases.xlsx
+++ b/Test cases.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Smoke Test Cases" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,9 +18,246 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="60">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Precondition</t>
+  </si>
+  <si>
+    <t>Test Steps</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Remark</t>
+  </si>
+  <si>
+    <t>Check website logo is displayed correctly</t>
+  </si>
+  <si>
+    <t>Check website logo links to homepage</t>
+  </si>
+  <si>
+    <t>Homepage elements</t>
+  </si>
+  <si>
+    <t>Main Navigation Menu</t>
+  </si>
+  <si>
+    <t>Product Listing Page</t>
+  </si>
+  <si>
+    <t>Product Detail Page</t>
+  </si>
+  <si>
+    <t>Cart</t>
+  </si>
+  <si>
+    <t>Checkout</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Contact Us Form</t>
+  </si>
+  <si>
+    <t>Social Media</t>
+  </si>
+  <si>
+    <t>Check main menu Home category is functional</t>
+  </si>
+  <si>
+    <t>Check main menu Apparel &amp; Accessories category is functional</t>
+  </si>
+  <si>
+    <t>Check main menu Makeup category is functional</t>
+  </si>
+  <si>
+    <t>Check main menu Skincare category is functional</t>
+  </si>
+  <si>
+    <t>Check main menu Fragrance category is functional</t>
+  </si>
+  <si>
+    <t>Check main menu Men category is functional</t>
+  </si>
+  <si>
+    <t>Check main menu Hair Care category is functional</t>
+  </si>
+  <si>
+    <t>Check main menu Books category is functional</t>
+  </si>
+  <si>
+    <t>Check Header Social Media links are working</t>
+  </si>
+  <si>
+    <t>Check Footer Social Media links are working</t>
+  </si>
+  <si>
+    <t>Guest</t>
+  </si>
+  <si>
+    <t>Member</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>1. Open https://abantecart.codifyme.co.nz
+2. Check if all block elements are displayed:
+• Header - headerstrip 
+• Header - headerdetails
+• categorymenu (main navigation menu)
+• slider
+• Maincontainer - promo_section
+• Maincontainer - featured
+• Maincontainer - latest
+• Maincontainer - bestseller
+• Maincontainer - special
+• Maincontainer - banner
+• Maincontainer - popularbrands
+• Footer - footersocial
+• Footer - footerlinks
+• Footer - copyrightbottom</t>
+  </si>
+  <si>
+    <t>1. Open https://abantecart.codifyme.co.nz
+2. Click Login or register
+3. Enter Login Name and Password
+4. Click Login
+5. Click Logoff</t>
+  </si>
+  <si>
+    <t>5. My Account Information page should appear.
+6. "Success: Your account has been successfully updated." should appear.</t>
+  </si>
+  <si>
+    <t>1. Open https://abantecart.codifyme.co.nz
+2. Click Login or register
+3. Enter Login Name and Password
+4. Click Login
+5. Click Edit account details
+6. Change First Name, Last Name and Telephone
+7. Click Continue</t>
+  </si>
+  <si>
+    <t>2.) All block elements should be displayed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open https://abantecart.codifyme.co.nz
+2. 
+3. </t>
+  </si>
+  <si>
+    <t>2. Logo exists in specified Url.</t>
+  </si>
+  <si>
+    <t>2. Homepage reloads.</t>
+  </si>
+  <si>
+    <t>1. Open https://abantecart.codifyme.co.nz
+2. Click website logo</t>
+  </si>
+  <si>
+    <t>1. Open https://abantecart.codifyme.co.nz
+2. Test logo exists in the Url specified</t>
+  </si>
+  <si>
+    <t>Check user can login and logout</t>
+  </si>
+  <si>
+    <t>Check user can change Personal details</t>
+  </si>
+  <si>
+    <t>Check all Homepage block elements are displayed</t>
+  </si>
+  <si>
+    <t>Check user can search using a valid query</t>
+  </si>
+  <si>
+    <t>Check user can search using an invalid query</t>
+  </si>
+  <si>
+    <t>Check user can search using an empty field</t>
+  </si>
+  <si>
+    <t>Check user can submit an enquiry</t>
+  </si>
+  <si>
+    <t>Check all PLP block elements are displayed:
+• heading1
+• top sorting well
+• thumbnails grid
+• bottom sorting well</t>
+  </si>
+  <si>
+    <t>Check all PDP block elements are displayed:
+• Latest products
+• thumbnails
+• mainimage
+• productname
+• productprice
+• quantitybox
+• total price
+• Add to Cart button
+• Buy Now button
+• Description tab</t>
+  </si>
+  <si>
+    <t>Check user can remove product from cart</t>
+  </si>
+  <si>
+    <t>Check user can checkout</t>
+  </si>
+  <si>
+    <t>Check user can add products to cart from PLP</t>
+  </si>
+  <si>
+    <t>Check user can add products to cart from PDP</t>
+  </si>
+  <si>
+    <t>1. Open https://abantecart.codifyme.co.nz
+2. Mouseover HOME 
+3. Click HOME</t>
+  </si>
+  <si>
+    <t>2. Menu appears with links to: Specials, Account, Cart, Checkout.
+3. Homepage reloads.</t>
+  </si>
+  <si>
+    <t>1. Open https://abantecart.codifyme.co.nz
+2. Mouseover APPAREL &amp; ACCESSORIES
+3. Click APPAREL &amp; ACCESSORIES</t>
+  </si>
+  <si>
+    <t>2. Menu appears with links to: Shoes, T-shirts.
+3. APPAREL &amp; ACCESSORIES category page appears.</t>
+  </si>
+  <si>
+    <t>2. Account Login page appears.
+4. My Account page appears with Welcome back message.
+5. Account Logout page appears.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,13 +265,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,13 +297,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -331,12 +593,444 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" style="2" customWidth="1"/>
+    <col min="3" max="3" width="55.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="52.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="31.5703125" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="240" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="165" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="3"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="3"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding test case: Check user can change Personal details
</commit_message>
<xml_diff>
--- a/Test cases.xlsx
+++ b/Test cases.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="61">
   <si>
     <t>ID</t>
   </si>
@@ -112,9 +112,6 @@
   </si>
   <si>
     <t>Member</t>
-  </si>
-  <si>
-    <t>Account</t>
   </si>
   <si>
     <t>1. Open https://abantecart.codifyme.co.nz
@@ -142,19 +139,6 @@
 5. Click Logoff</t>
   </si>
   <si>
-    <t>5. My Account Information page should appear.
-6. "Success: Your account has been successfully updated." should appear.</t>
-  </si>
-  <si>
-    <t>1. Open https://abantecart.codifyme.co.nz
-2. Click Login or register
-3. Enter Login Name and Password
-4. Click Login
-5. Click Edit account details
-6. Change First Name, Last Name and Telephone
-7. Click Continue</t>
-  </si>
-  <si>
     <t>2.) All block elements should be displayed.</t>
   </si>
   <si>
@@ -251,6 +235,31 @@
     <t>2. Account Login page appears.
 4. My Account page appears with Welcome back message.
 5. Account Logout page appears.</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>My Account</t>
+  </si>
+  <si>
+    <t>1. Open https://abantecart.codifyme.co.nz
+2. Click Account &gt; Login
+3. Enter Login Name and Password
+4. Click Login
+5. Click Edit account details
+6. Change First Name, Last Name and Telephone
+7. Click Continue
+8. Click Edit account details</t>
+  </si>
+  <si>
+    <t>5. My Account Information page should appear.
+7. Expected as follows:
+• "Success: Your account has been successfully updated." should appear. 
+• Name beside My Account header updates with new name.
+8. Your Personal Details shows updated details
+• Welcome back message reflects new name.
+8. My Acount Information page appears with correct field values.</t>
   </si>
 </sst>
 </file>
@@ -597,7 +606,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,33 +651,33 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="210" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="240" x14ac:dyDescent="0.25">
@@ -679,16 +688,16 @@
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -705,10 +714,10 @@
         <v>29</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -725,10 +734,10 @@
         <v>29</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -745,10 +754,10 @@
         <v>29</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -765,10 +774,10 @@
         <v>29</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -785,7 +794,7 @@
         <v>29</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -866,7 +875,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>29</v>
@@ -880,7 +889,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>29</v>
@@ -894,7 +903,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>29</v>
@@ -936,7 +945,7 @@
         <v>17</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>29</v>
@@ -950,7 +959,7 @@
         <v>12</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>29</v>
@@ -964,7 +973,7 @@
         <v>13</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>29</v>
@@ -978,7 +987,7 @@
         <v>14</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>30</v>
@@ -992,7 +1001,7 @@
         <v>14</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1003,7 +1012,7 @@
         <v>14</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>30</v>
@@ -1017,7 +1026,7 @@
         <v>15</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Adding Check all Homepage block elements are displayed test script
</commit_message>
<xml_diff>
--- a/Test cases.xlsx
+++ b/Test cases.xlsx
@@ -266,18 +266,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -306,11 +298,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -318,12 +309,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -602,11 +589,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,9 +601,9 @@
     <col min="1" max="1" width="2.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" style="2" customWidth="1"/>
     <col min="3" max="3" width="55.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.7109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="52.140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="31.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="42" style="2" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -663,7 +650,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="210" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1031,12 +1018,6 @@
       <c r="D26" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C33" s="3"/>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C34" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding Check website logo is displayed correctly script
</commit_message>
<xml_diff>
--- a/Test cases.xlsx
+++ b/Test cases.xlsx
@@ -147,18 +147,11 @@
 3. </t>
   </si>
   <si>
-    <t>2. Logo exists in specified Url.</t>
-  </si>
-  <si>
     <t>2. Homepage reloads.</t>
   </si>
   <si>
     <t>1. Open https://abantecart.codifyme.co.nz
 2. Click website logo</t>
-  </si>
-  <si>
-    <t>1. Open https://abantecart.codifyme.co.nz
-2. Test logo exists in the Url specified</t>
   </si>
   <si>
     <t>Check user can login and logout</t>
@@ -260,6 +253,15 @@
 8. Your Personal Details shows updated details
 • Welcome back message reflects new name.
 8. My Acount Information page appears with correct field values.</t>
+  </si>
+  <si>
+    <t>1. Open https://abantecart.codifyme.co.nz
+2. Check if logo element is displayed
+3. Check if logo image exists in the specified source Url</t>
+  </si>
+  <si>
+    <t>2. Logo element should be displayed
+3. Logo image file exists in the specified source Url.</t>
   </si>
 </sst>
 </file>
@@ -591,9 +593,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,16 +640,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="180" x14ac:dyDescent="0.25">
@@ -655,16 +657,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="240" x14ac:dyDescent="0.25">
@@ -675,7 +677,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>29</v>
@@ -687,7 +689,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -701,10 +703,10 @@
         <v>29</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -721,10 +723,10 @@
         <v>29</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -741,10 +743,10 @@
         <v>29</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -761,10 +763,10 @@
         <v>29</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -862,7 +864,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>29</v>
@@ -876,7 +878,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>29</v>
@@ -890,7 +892,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>29</v>
@@ -932,7 +934,7 @@
         <v>17</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>29</v>
@@ -946,7 +948,7 @@
         <v>12</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>29</v>
@@ -960,7 +962,7 @@
         <v>13</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>29</v>
@@ -974,7 +976,7 @@
         <v>14</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>30</v>
@@ -988,7 +990,7 @@
         <v>14</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -999,7 +1001,7 @@
         <v>14</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>30</v>
@@ -1013,7 +1015,7 @@
         <v>15</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
additional assertion for 'Check website logo is displayed correctly' test case
</commit_message>
<xml_diff>
--- a/Test cases.xlsx
+++ b/Test cases.xlsx
@@ -48,9 +48,6 @@
     <t>Check website logo is displayed correctly</t>
   </si>
   <si>
-    <t>Check website logo links to homepage</t>
-  </si>
-  <si>
     <t>Homepage elements</t>
   </si>
   <si>
@@ -147,13 +144,6 @@
 3. </t>
   </si>
   <si>
-    <t>2. Homepage reloads.</t>
-  </si>
-  <si>
-    <t>1. Open https://abantecart.codifyme.co.nz
-2. Click website logo</t>
-  </si>
-  <si>
     <t>Check user can login and logout</t>
   </si>
   <si>
@@ -255,23 +245,44 @@
 8. My Acount Information page appears with correct field values.</t>
   </si>
   <si>
+    <t>Check website logo links to homepage on the same tab</t>
+  </si>
+  <si>
     <t>1. Open https://abantecart.codifyme.co.nz
 2. Check if logo element is displayed
-3. Check if logo image exists in the specified source Url</t>
-  </si>
-  <si>
-    <t>2. Logo element should be displayed
-3. Logo image file exists in the specified source Url.</t>
+3. Check if logo image src URL is correct
+4. Check if logo image exists in the specified source URL</t>
+  </si>
+  <si>
+    <t>2. Logo element should be displayed.
+3. Logo image src URL should be "resources/image/18/73/3.png".
+4. Logo image file exists in the specified source URL.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open https://abantecart.codifyme.co.nz
+2. Check if logo have correct link
+3. Check if logo opens only on the same tab </t>
+  </si>
+  <si>
+    <t>2. Logo href URL should be "https://abantecart.codifyme.co.nz/".
+3. HTML link tag should not have target and onclick attributes.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -303,12 +314,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -593,9 +607,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,7 +617,7 @@
     <col min="1" max="1" width="2.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" style="2" customWidth="1"/>
     <col min="3" max="3" width="55.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="63.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="52.140625" style="2" customWidth="1"/>
     <col min="6" max="6" width="42" style="2" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="2"/>
@@ -635,98 +649,98 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="3" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="2" t="s">
+    </row>
+    <row r="4" spans="1:8" s="3" customFormat="1" ht="240" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="180" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="2" t="s">
+    </row>
+    <row r="5" spans="1:8" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F5" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="240" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -734,19 +748,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -754,19 +768,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -774,16 +788,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -791,13 +805,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -805,13 +819,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -819,13 +833,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -833,13 +847,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -847,13 +861,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -861,13 +875,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -875,13 +889,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -889,13 +903,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -903,13 +917,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -917,13 +931,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -931,13 +945,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -945,13 +959,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="165" x14ac:dyDescent="0.25">
@@ -959,13 +973,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -973,13 +987,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -987,10 +1001,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -998,13 +1012,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1012,13 +1026,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 'Check website logo links to homepage on the same tab' test script
</commit_message>
<xml_diff>
--- a/Test cases.xlsx
+++ b/Test cases.xlsx
@@ -609,7 +609,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,22 +724,22 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="D6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added 'Check main menu Home category is functional' test script
</commit_message>
<xml_diff>
--- a/Test cases.xlsx
+++ b/Test cases.xlsx
@@ -198,15 +198,6 @@
   </si>
   <si>
     <t>1. Open https://abantecart.codifyme.co.nz
-2. Mouseover HOME 
-3. Click HOME</t>
-  </si>
-  <si>
-    <t>2. Menu appears with links to: Specials, Account, Cart, Checkout.
-3. Homepage reloads.</t>
-  </si>
-  <si>
-    <t>1. Open https://abantecart.codifyme.co.nz
 2. Mouseover APPAREL &amp; ACCESSORIES
 3. Click APPAREL &amp; ACCESSORIES</t>
   </si>
@@ -266,6 +257,16 @@
   <si>
     <t>2. Logo href URL should be "https://abantecart.codifyme.co.nz/".
 3. HTML link tag should not have target and onclick attributes.</t>
+  </si>
+  <si>
+    <t>2. HOME Menu button link should be working.
+3. All links should be working.</t>
+  </si>
+  <si>
+    <t>1. Open https://abantecart.codifyme.co.nz
+2. Check if HOME Menu link is working
+3. Mouseover HOME Menu
+3. Check if all links in the HOME Menu dropdown are working</t>
   </si>
 </sst>
 </file>
@@ -608,8 +609,8 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,7 +655,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>34</v>
@@ -663,7 +664,7 @@
         <v>31</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="3" customFormat="1" ht="180" x14ac:dyDescent="0.25">
@@ -671,16 +672,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="3" customFormat="1" ht="240" x14ac:dyDescent="0.25">
@@ -717,10 +718,10 @@
         <v>28</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -731,36 +732,36 @@
         <v>9</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -777,10 +778,10 @@
         <v>28</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added 'Check main menu Apparel & Accessories category is functional' test script
</commit_message>
<xml_diff>
--- a/Test cases.xlsx
+++ b/Test cases.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
   <si>
     <t>ID</t>
   </si>
@@ -139,11 +139,6 @@
     <t>2.) All block elements should be displayed.</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Open https://abantecart.codifyme.co.nz
-2. 
-3. </t>
-  </si>
-  <si>
     <t>Check user can login and logout</t>
   </si>
   <si>
@@ -197,15 +192,6 @@
     <t>Check user can add products to cart from PDP</t>
   </si>
   <si>
-    <t>1. Open https://abantecart.codifyme.co.nz
-2. Mouseover APPAREL &amp; ACCESSORIES
-3. Click APPAREL &amp; ACCESSORIES</t>
-  </si>
-  <si>
-    <t>2. Menu appears with links to: Shoes, T-shirts.
-3. APPAREL &amp; ACCESSORIES category page appears.</t>
-  </si>
-  <si>
     <t>2. Account Login page appears.
 4. My Account page appears with Welcome back message.
 5. Account Logout page appears.</t>
@@ -259,14 +245,27 @@
 3. HTML link tag should not have target and onclick attributes.</t>
   </si>
   <si>
-    <t>2. HOME Menu button link should be working.
-3. All links should be working.</t>
-  </si>
-  <si>
     <t>1. Open https://abantecart.codifyme.co.nz
 2. Check if HOME Menu link is working
 3. Mouseover HOME Menu
-3. Check if all links in the HOME Menu dropdown are working</t>
+4. Check if all links in the HOME Menu dropdown are working</t>
+  </si>
+  <si>
+    <t>1. Open https://abantecart.codifyme.co.nz
+2. Check if APPAREL &amp; ACCESSORIES Menu link is working
+3. Mouseover APPAREL &amp; ACCESSORIES Menu
+4. Check if all links in the APPAREL &amp; ACCESSORIES Menu dropdown are working</t>
+  </si>
+  <si>
+    <t>2. APPAREL &amp; ACCESSORIES Menu button link should be working.
+3. Dropdown appears .
+4. All dropdown links should be working.</t>
+  </si>
+  <si>
+    <t>2. HOME Menu button link should be working.
+should be working.
+3. Dropdown appears .
+4. All dropdown links should be working.</t>
   </si>
 </sst>
 </file>
@@ -610,7 +609,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,16 +654,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>31</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="3" customFormat="1" ht="180" x14ac:dyDescent="0.25">
@@ -672,16 +671,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="3" customFormat="1" ht="240" x14ac:dyDescent="0.25">
@@ -692,7 +691,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>28</v>
@@ -718,10 +717,10 @@
         <v>28</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -732,16 +731,16 @@
         <v>9</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="F6" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -758,33 +757,33 @@
         <v>28</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+    <row r="8" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="D8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -796,9 +795,6 @@
       </c>
       <c r="D9" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -879,7 +875,7 @@
         <v>15</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>28</v>
@@ -893,7 +889,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>28</v>
@@ -907,7 +903,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>28</v>
@@ -949,7 +945,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>28</v>
@@ -963,7 +959,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>28</v>
@@ -977,7 +973,7 @@
         <v>12</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>28</v>
@@ -991,7 +987,7 @@
         <v>13</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>29</v>
@@ -1005,7 +1001,7 @@
         <v>13</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1016,7 +1012,7 @@
         <v>13</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>29</v>
@@ -1030,7 +1026,7 @@
         <v>14</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Added 'Check main menu Skincare category is functional' test script
</commit_message>
<xml_diff>
--- a/Test cases.xlsx
+++ b/Test cases.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="72">
   <si>
     <t>ID</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>Check Footer Social Media links are working</t>
-  </si>
-  <si>
-    <t>Guest</t>
   </si>
   <si>
     <t>Member</t>
@@ -264,6 +261,75 @@
   <si>
     <t>2. HOME Menu button link should be working.
 should be working.
+3. Dropdown appears .
+4. All dropdown links should be working.</t>
+  </si>
+  <si>
+    <t>1. Open https://abantecart.codifyme.co.nz
+2. Check if MAKEUP Menu link is working
+3. Mouseover MAKEUP Menu
+4. Check if all links in the MAKEUP Menu dropdown are working</t>
+  </si>
+  <si>
+    <t>2. MAKEUP Menu button link should be working.
+3. Dropdown appears .
+4. All dropdown links should be working.</t>
+  </si>
+  <si>
+    <t>Guest user</t>
+  </si>
+  <si>
+    <t>1. Open https://abantecart.codifyme.co.nz
+2. Check if SKINCARE Menu link is working
+3. Mouseover SKINCARE Menu
+4. Check if all links in the SKINCARE Menu dropdown are working</t>
+  </si>
+  <si>
+    <t>2. SKINCARE Menu button link should be working.
+3. Dropdown appears .
+4. All dropdown links should be working.</t>
+  </si>
+  <si>
+    <t>1. Open https://abantecart.codifyme.co.nz
+2. Check if FRAGRANCE Menu link is working
+3. Mouseover FRAGRANCE Menu
+4. Check if all links in the FRAGRANCE Menu dropdown are working</t>
+  </si>
+  <si>
+    <t>2. FRAGRANCE Menu button link should be working.
+3. Dropdown appears .
+4. All dropdown links should be working.</t>
+  </si>
+  <si>
+    <t>1. Open https://abantecart.codifyme.co.nz
+2. Check if MEN Menu link is working
+3. Mouseover MEN Menu
+4. Check if all links in the MEN Menu dropdown are working</t>
+  </si>
+  <si>
+    <t>2. MEN Menu button link should be working.
+3. Dropdown appears .
+4. All dropdown links should be working.</t>
+  </si>
+  <si>
+    <t>1. Open https://abantecart.codifyme.co.nz
+2. Check if HAIR CARE Menu link is working
+3. Mouseover HAIR CARE Menu
+4. Check if all links in the HAIR CARE Menu dropdown are working</t>
+  </si>
+  <si>
+    <t>2. HAIR CARE Menu button link should be working.
+3. Dropdown appears .
+4. All dropdown links should be working.</t>
+  </si>
+  <si>
+    <t>1. Open https://abantecart.codifyme.co.nz
+2. Check if BOOKS Menu link is working
+3. Mouseover BOOKS Menu
+4. Check if all links in the BOOKS Menu dropdown are working</t>
+  </si>
+  <si>
+    <t>2. BOOKS Menu button link should be working.
 3. Dropdown appears .
 4. All dropdown links should be working.</t>
   </si>
@@ -608,7 +674,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -654,16 +720,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="3" customFormat="1" ht="180" x14ac:dyDescent="0.25">
@@ -671,16 +737,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="3" customFormat="1" ht="240" x14ac:dyDescent="0.25">
@@ -691,16 +757,16 @@
         <v>9</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -714,13 +780,13 @@
         <v>8</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -731,16 +797,16 @@
         <v>9</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -754,13 +820,13 @@
         <v>18</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -774,44 +840,56 @@
         <v>19</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+    </row>
+    <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="D9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -822,10 +900,16 @@
         <v>22</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -836,10 +920,16 @@
         <v>23</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -850,10 +940,16 @@
         <v>24</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -864,7 +960,13 @@
         <v>25</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>28</v>
+        <v>61</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -875,10 +977,10 @@
         <v>15</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -889,10 +991,10 @@
         <v>15</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -903,10 +1005,10 @@
         <v>15</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -920,7 +1022,7 @@
         <v>26</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -934,7 +1036,7 @@
         <v>27</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -945,10 +1047,10 @@
         <v>16</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -959,10 +1061,10 @@
         <v>11</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="165" x14ac:dyDescent="0.25">
@@ -973,10 +1075,10 @@
         <v>12</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -987,10 +1089,10 @@
         <v>13</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1001,7 +1103,7 @@
         <v>13</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1012,10 +1114,10 @@
         <v>13</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1026,10 +1128,10 @@
         <v>14</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 'Check main menu Fragrance category is functional' test script
</commit_message>
<xml_diff>
--- a/Test cases.xlsx
+++ b/Test cases.xlsx
@@ -675,7 +675,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,22 +890,22 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11" s="2" t="s">
+      <c r="D11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="3" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added 'Check main menu Men category is functional' test script
</commit_message>
<xml_diff>
--- a/Test cases.xlsx
+++ b/Test cases.xlsx
@@ -910,22 +910,22 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E12" s="2" t="s">
+      <c r="D12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="3" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added 'Check main menu Hair Care category is functional' test script
</commit_message>
<xml_diff>
--- a/Test cases.xlsx
+++ b/Test cases.xlsx
@@ -675,7 +675,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,22 +930,22 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E13" s="2" t="s">
+      <c r="D13" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="3" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added 'Check main menu Books category is functional' test script
</commit_message>
<xml_diff>
--- a/Test cases.xlsx
+++ b/Test cases.xlsx
@@ -675,7 +675,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,22 +950,22 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" s="2" t="s">
+      <c r="D14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="3" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added 'Check user can search a keyword that matches search criteria' test script
</commit_message>
<xml_diff>
--- a/Test cases.xlsx
+++ b/Test cases.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="97">
   <si>
     <t>ID</t>
   </si>
@@ -145,15 +145,6 @@
     <t>Check all Homepage block elements are displayed</t>
   </si>
   <si>
-    <t>Check user can search using a valid query</t>
-  </si>
-  <si>
-    <t>Check user can search using an invalid query</t>
-  </si>
-  <si>
-    <t>Check user can search using an empty field</t>
-  </si>
-  <si>
     <t>Check user can submit an enquiry</t>
   </si>
   <si>
@@ -332,6 +323,96 @@
     <t>2. BOOKS Menu button link should be working.
 3. Dropdown appears .
 4. All dropdown links should be working.</t>
+  </si>
+  <si>
+    <t>3. Search page appears with search results
+5. Search page appears with search results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open https://abantecart.codifyme.co.nz
+2. Enter search keyword on header search box
+3. Click magnifying lens button
+4. Enter another valid search keyword on the Search page
+5. Click Search button
+</t>
+  </si>
+  <si>
+    <t>Check user can search a keyword that matches search criteria</t>
+  </si>
+  <si>
+    <t>Check user cannot search a keyword that does not match search criteria</t>
+  </si>
+  <si>
+    <t>3A</t>
+  </si>
+  <si>
+    <t>3B</t>
+  </si>
+  <si>
+    <t>3C</t>
+  </si>
+  <si>
+    <t>4A</t>
+  </si>
+  <si>
+    <t>4B</t>
+  </si>
+  <si>
+    <t>4C</t>
+  </si>
+  <si>
+    <t>4D</t>
+  </si>
+  <si>
+    <t>4E</t>
+  </si>
+  <si>
+    <t>4F</t>
+  </si>
+  <si>
+    <t>4G</t>
+  </si>
+  <si>
+    <t>4H</t>
+  </si>
+  <si>
+    <t>5A</t>
+  </si>
+  <si>
+    <t>5B</t>
+  </si>
+  <si>
+    <t>6A</t>
+  </si>
+  <si>
+    <t>6B</t>
+  </si>
+  <si>
+    <t>8A</t>
+  </si>
+  <si>
+    <t>8B</t>
+  </si>
+  <si>
+    <t>9A</t>
+  </si>
+  <si>
+    <t>9B</t>
+  </si>
+  <si>
+    <t>9C</t>
+  </si>
+  <si>
+    <t>1A</t>
+  </si>
+  <si>
+    <t>2A</t>
+  </si>
+  <si>
+    <t>7A</t>
+  </si>
+  <si>
+    <t>10A</t>
   </si>
 </sst>
 </file>
@@ -671,16 +752,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" style="2" customWidth="1"/>
     <col min="3" max="3" width="55.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
@@ -716,11 +797,11 @@
       </c>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>1</v>
+      <c r="A2" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>32</v>
@@ -729,29 +810,29 @@
         <v>30</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="3" customFormat="1" ht="180" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>2</v>
+      <c r="A3" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>33</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="3" customFormat="1" ht="240" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>3</v>
+      <c r="A4" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>9</v>
@@ -760,7 +841,7 @@
         <v>34</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>29</v>
@@ -770,8 +851,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>4</v>
+      <c r="A5" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>9</v>
@@ -780,38 +861,38 @@
         <v>8</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>5</v>
+      <c r="A6" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="F6" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>6</v>
+      <c r="A7" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>10</v>
@@ -820,18 +901,18 @@
         <v>18</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="8" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>7</v>
+      <c r="A8" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>10</v>
@@ -840,18 +921,18 @@
         <v>19</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>8</v>
+      <c r="A9" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>10</v>
@@ -860,18 +941,18 @@
         <v>20</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>9</v>
+      <c r="A10" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>10</v>
@@ -880,18 +961,18 @@
         <v>21</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>10</v>
+      <c r="A11" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>10</v>
@@ -900,18 +981,18 @@
         <v>22</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="F11" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>11</v>
+      <c r="A12" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>10</v>
@@ -920,18 +1001,18 @@
         <v>23</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>12</v>
+      <c r="A13" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>10</v>
@@ -940,18 +1021,18 @@
         <v>24</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>13</v>
+      <c r="A14" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>10</v>
@@ -960,177 +1041,169 @@
         <v>25</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E14" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>15</v>
+      <c r="F15" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>16</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>17</v>
+      <c r="A18" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>18</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>19</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>20</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="165" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="165" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>21</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>22</v>
+      <c r="A23" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>23</v>
+      <c r="A24" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>24</v>
+        <v>38</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>25</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26" s="2" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added 'Check user cannot search a keyword that does not match search criteria' test script
</commit_message>
<xml_diff>
--- a/Test cases.xlsx
+++ b/Test cases.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="99">
   <si>
     <t>ID</t>
   </si>
@@ -201,218 +201,230 @@
 8. Click Edit account details</t>
   </si>
   <si>
+    <t>Check website logo links to homepage on the same tab</t>
+  </si>
+  <si>
+    <t>1. Open https://abantecart.codifyme.co.nz
+2. Check if logo element is displayed
+3. Check if logo image src URL is correct
+4. Check if logo image exists in the specified source URL</t>
+  </si>
+  <si>
+    <t>2. Logo element should be displayed.
+3. Logo image src URL should be "resources/image/18/73/3.png".
+4. Logo image file exists in the specified source URL.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open https://abantecart.codifyme.co.nz
+2. Check if logo have correct link
+3. Check if logo opens only on the same tab </t>
+  </si>
+  <si>
+    <t>2. Logo href URL should be "https://abantecart.codifyme.co.nz/".
+3. HTML link tag should not have target and onclick attributes.</t>
+  </si>
+  <si>
+    <t>1. Open https://abantecart.codifyme.co.nz
+2. Check if HOME Menu link is working
+3. Mouseover HOME Menu
+4. Check if all links in the HOME Menu dropdown are working</t>
+  </si>
+  <si>
+    <t>1. Open https://abantecart.codifyme.co.nz
+2. Check if APPAREL &amp; ACCESSORIES Menu link is working
+3. Mouseover APPAREL &amp; ACCESSORIES Menu
+4. Check if all links in the APPAREL &amp; ACCESSORIES Menu dropdown are working</t>
+  </si>
+  <si>
+    <t>2. APPAREL &amp; ACCESSORIES Menu button link should be working.
+3. Dropdown appears .
+4. All dropdown links should be working.</t>
+  </si>
+  <si>
+    <t>2. HOME Menu button link should be working.
+should be working.
+3. Dropdown appears .
+4. All dropdown links should be working.</t>
+  </si>
+  <si>
+    <t>1. Open https://abantecart.codifyme.co.nz
+2. Check if MAKEUP Menu link is working
+3. Mouseover MAKEUP Menu
+4. Check if all links in the MAKEUP Menu dropdown are working</t>
+  </si>
+  <si>
+    <t>2. MAKEUP Menu button link should be working.
+3. Dropdown appears .
+4. All dropdown links should be working.</t>
+  </si>
+  <si>
+    <t>Guest user</t>
+  </si>
+  <si>
+    <t>1. Open https://abantecart.codifyme.co.nz
+2. Check if SKINCARE Menu link is working
+3. Mouseover SKINCARE Menu
+4. Check if all links in the SKINCARE Menu dropdown are working</t>
+  </si>
+  <si>
+    <t>2. SKINCARE Menu button link should be working.
+3. Dropdown appears .
+4. All dropdown links should be working.</t>
+  </si>
+  <si>
+    <t>1. Open https://abantecart.codifyme.co.nz
+2. Check if FRAGRANCE Menu link is working
+3. Mouseover FRAGRANCE Menu
+4. Check if all links in the FRAGRANCE Menu dropdown are working</t>
+  </si>
+  <si>
+    <t>2. FRAGRANCE Menu button link should be working.
+3. Dropdown appears .
+4. All dropdown links should be working.</t>
+  </si>
+  <si>
+    <t>1. Open https://abantecart.codifyme.co.nz
+2. Check if MEN Menu link is working
+3. Mouseover MEN Menu
+4. Check if all links in the MEN Menu dropdown are working</t>
+  </si>
+  <si>
+    <t>2. MEN Menu button link should be working.
+3. Dropdown appears .
+4. All dropdown links should be working.</t>
+  </si>
+  <si>
+    <t>1. Open https://abantecart.codifyme.co.nz
+2. Check if HAIR CARE Menu link is working
+3. Mouseover HAIR CARE Menu
+4. Check if all links in the HAIR CARE Menu dropdown are working</t>
+  </si>
+  <si>
+    <t>2. HAIR CARE Menu button link should be working.
+3. Dropdown appears .
+4. All dropdown links should be working.</t>
+  </si>
+  <si>
+    <t>1. Open https://abantecart.codifyme.co.nz
+2. Check if BOOKS Menu link is working
+3. Mouseover BOOKS Menu
+4. Check if all links in the BOOKS Menu dropdown are working</t>
+  </si>
+  <si>
+    <t>2. BOOKS Menu button link should be working.
+3. Dropdown appears .
+4. All dropdown links should be working.</t>
+  </si>
+  <si>
+    <t>3. Search page appears with search results
+5. Search page appears with search results</t>
+  </si>
+  <si>
+    <t>Check user can search a keyword that matches search criteria</t>
+  </si>
+  <si>
+    <t>Check user cannot search a keyword that does not match search criteria</t>
+  </si>
+  <si>
+    <t>3A</t>
+  </si>
+  <si>
+    <t>3B</t>
+  </si>
+  <si>
+    <t>3C</t>
+  </si>
+  <si>
+    <t>4A</t>
+  </si>
+  <si>
+    <t>4B</t>
+  </si>
+  <si>
+    <t>4C</t>
+  </si>
+  <si>
+    <t>4D</t>
+  </si>
+  <si>
+    <t>4E</t>
+  </si>
+  <si>
+    <t>4F</t>
+  </si>
+  <si>
+    <t>4G</t>
+  </si>
+  <si>
+    <t>4H</t>
+  </si>
+  <si>
+    <t>5A</t>
+  </si>
+  <si>
+    <t>5B</t>
+  </si>
+  <si>
+    <t>6A</t>
+  </si>
+  <si>
+    <t>6B</t>
+  </si>
+  <si>
+    <t>8A</t>
+  </si>
+  <si>
+    <t>8B</t>
+  </si>
+  <si>
+    <t>9A</t>
+  </si>
+  <si>
+    <t>9B</t>
+  </si>
+  <si>
+    <t>9C</t>
+  </si>
+  <si>
+    <t>1A</t>
+  </si>
+  <si>
+    <t>2A</t>
+  </si>
+  <si>
+    <t>7A</t>
+  </si>
+  <si>
+    <t>10A</t>
+  </si>
+  <si>
     <t>5. My Account Information page should appear.
 7. Expected as follows:
 • "Success: Your account has been successfully updated." should appear. 
 • Name beside My Account header updates with new name.
 8. Your Personal Details shows updated details
 • Welcome back message reflects new name.
-8. My Acount Information page appears with correct field values.</t>
-  </si>
-  <si>
-    <t>Check website logo links to homepage on the same tab</t>
-  </si>
-  <si>
-    <t>1. Open https://abantecart.codifyme.co.nz
-2. Check if logo element is displayed
-3. Check if logo image src URL is correct
-4. Check if logo image exists in the specified source URL</t>
-  </si>
-  <si>
-    <t>2. Logo element should be displayed.
-3. Logo image src URL should be "resources/image/18/73/3.png".
-4. Logo image file exists in the specified source URL.</t>
+8. My Account Information page appears with correct field values.</t>
   </si>
   <si>
     <t xml:space="preserve">1. Open https://abantecart.codifyme.co.nz
-2. Check if logo have correct link
-3. Check if logo opens only on the same tab </t>
-  </si>
-  <si>
-    <t>2. Logo href URL should be "https://abantecart.codifyme.co.nz/".
-3. HTML link tag should not have target and onclick attributes.</t>
-  </si>
-  <si>
-    <t>1. Open https://abantecart.codifyme.co.nz
-2. Check if HOME Menu link is working
-3. Mouseover HOME Menu
-4. Check if all links in the HOME Menu dropdown are working</t>
-  </si>
-  <si>
-    <t>1. Open https://abantecart.codifyme.co.nz
-2. Check if APPAREL &amp; ACCESSORIES Menu link is working
-3. Mouseover APPAREL &amp; ACCESSORIES Menu
-4. Check if all links in the APPAREL &amp; ACCESSORIES Menu dropdown are working</t>
-  </si>
-  <si>
-    <t>2. APPAREL &amp; ACCESSORIES Menu button link should be working.
-3. Dropdown appears .
-4. All dropdown links should be working.</t>
-  </si>
-  <si>
-    <t>2. HOME Menu button link should be working.
-should be working.
-3. Dropdown appears .
-4. All dropdown links should be working.</t>
-  </si>
-  <si>
-    <t>1. Open https://abantecart.codifyme.co.nz
-2. Check if MAKEUP Menu link is working
-3. Mouseover MAKEUP Menu
-4. Check if all links in the MAKEUP Menu dropdown are working</t>
-  </si>
-  <si>
-    <t>2. MAKEUP Menu button link should be working.
-3. Dropdown appears .
-4. All dropdown links should be working.</t>
-  </si>
-  <si>
-    <t>Guest user</t>
-  </si>
-  <si>
-    <t>1. Open https://abantecart.codifyme.co.nz
-2. Check if SKINCARE Menu link is working
-3. Mouseover SKINCARE Menu
-4. Check if all links in the SKINCARE Menu dropdown are working</t>
-  </si>
-  <si>
-    <t>2. SKINCARE Menu button link should be working.
-3. Dropdown appears .
-4. All dropdown links should be working.</t>
-  </si>
-  <si>
-    <t>1. Open https://abantecart.codifyme.co.nz
-2. Check if FRAGRANCE Menu link is working
-3. Mouseover FRAGRANCE Menu
-4. Check if all links in the FRAGRANCE Menu dropdown are working</t>
-  </si>
-  <si>
-    <t>2. FRAGRANCE Menu button link should be working.
-3. Dropdown appears .
-4. All dropdown links should be working.</t>
-  </si>
-  <si>
-    <t>1. Open https://abantecart.codifyme.co.nz
-2. Check if MEN Menu link is working
-3. Mouseover MEN Menu
-4. Check if all links in the MEN Menu dropdown are working</t>
-  </si>
-  <si>
-    <t>2. MEN Menu button link should be working.
-3. Dropdown appears .
-4. All dropdown links should be working.</t>
-  </si>
-  <si>
-    <t>1. Open https://abantecart.codifyme.co.nz
-2. Check if HAIR CARE Menu link is working
-3. Mouseover HAIR CARE Menu
-4. Check if all links in the HAIR CARE Menu dropdown are working</t>
-  </si>
-  <si>
-    <t>2. HAIR CARE Menu button link should be working.
-3. Dropdown appears .
-4. All dropdown links should be working.</t>
-  </si>
-  <si>
-    <t>1. Open https://abantecart.codifyme.co.nz
-2. Check if BOOKS Menu link is working
-3. Mouseover BOOKS Menu
-4. Check if all links in the BOOKS Menu dropdown are working</t>
-  </si>
-  <si>
-    <t>2. BOOKS Menu button link should be working.
-3. Dropdown appears .
-4. All dropdown links should be working.</t>
-  </si>
-  <si>
-    <t>3. Search page appears with search results
-5. Search page appears with search results</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Open https://abantecart.codifyme.co.nz
-2. Enter search keyword on header search box
+2. Enter a valid search keyword on header search box
 3. Click magnifying lens button
 4. Enter another valid search keyword on the Search page
 5. Click Search button
 </t>
   </si>
   <si>
-    <t>Check user can search a keyword that matches search criteria</t>
-  </si>
-  <si>
-    <t>Check user cannot search a keyword that does not match search criteria</t>
-  </si>
-  <si>
-    <t>3A</t>
-  </si>
-  <si>
-    <t>3B</t>
-  </si>
-  <si>
-    <t>3C</t>
-  </si>
-  <si>
-    <t>4A</t>
-  </si>
-  <si>
-    <t>4B</t>
-  </si>
-  <si>
-    <t>4C</t>
-  </si>
-  <si>
-    <t>4D</t>
-  </si>
-  <si>
-    <t>4E</t>
-  </si>
-  <si>
-    <t>4F</t>
-  </si>
-  <si>
-    <t>4G</t>
-  </si>
-  <si>
-    <t>4H</t>
-  </si>
-  <si>
-    <t>5A</t>
-  </si>
-  <si>
-    <t>5B</t>
-  </si>
-  <si>
-    <t>6A</t>
-  </si>
-  <si>
-    <t>6B</t>
-  </si>
-  <si>
-    <t>8A</t>
-  </si>
-  <si>
-    <t>8B</t>
-  </si>
-  <si>
-    <t>9A</t>
-  </si>
-  <si>
-    <t>9B</t>
-  </si>
-  <si>
-    <t>9C</t>
-  </si>
-  <si>
-    <t>1A</t>
-  </si>
-  <si>
-    <t>2A</t>
-  </si>
-  <si>
-    <t>7A</t>
-  </si>
-  <si>
-    <t>10A</t>
+    <t xml:space="preserve">1. Open https://abantecart.codifyme.co.nz
+2. Enter an invalid search keyword on header search box
+3. Click magnifying lens button
+4. Enter another invalid search keyword on the Search page
+5. Click Search button
+</t>
+  </si>
+  <si>
+    <t>3. Search results returns with no matches message
+5. Search results returns with no matches message</t>
   </si>
 </sst>
 </file>
@@ -755,8 +767,8 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,7 +810,7 @@
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>43</v>
@@ -815,7 +827,7 @@
     </row>
     <row r="3" spans="1:8" s="3" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>44</v>
@@ -827,12 +839,12 @@
         <v>45</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>46</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="3" customFormat="1" ht="240" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>9</v>
@@ -841,7 +853,7 @@
         <v>34</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>29</v>
@@ -852,7 +864,7 @@
     </row>
     <row r="5" spans="1:8" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>9</v>
@@ -861,38 +873,38 @@
         <v>8</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>10</v>
@@ -901,18 +913,18 @@
         <v>18</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>10</v>
@@ -921,18 +933,18 @@
         <v>19</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>10</v>
@@ -941,18 +953,18 @@
         <v>20</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>10</v>
@@ -961,18 +973,18 @@
         <v>21</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>10</v>
@@ -981,18 +993,18 @@
         <v>22</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>10</v>
@@ -1001,18 +1013,18 @@
         <v>23</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>10</v>
@@ -1021,18 +1033,18 @@
         <v>24</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>10</v>
@@ -1041,52 +1053,58 @@
         <v>25</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E14" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>58</v>
+      <c r="D16" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>17</v>
@@ -1095,12 +1113,12 @@
         <v>26</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>17</v>
@@ -1109,12 +1127,12 @@
         <v>27</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>16</v>
@@ -1123,12 +1141,12 @@
         <v>35</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>11</v>
@@ -1137,12 +1155,12 @@
         <v>36</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>12</v>
@@ -1151,12 +1169,12 @@
         <v>37</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>13</v>
@@ -1170,7 +1188,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>13</v>
@@ -1181,7 +1199,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>13</v>
@@ -1195,7 +1213,7 @@
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Added 'Check Header Social Media links are working' test script
</commit_message>
<xml_diff>
--- a/Test cases.xlsx
+++ b/Test cases.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="101">
   <si>
     <t>ID</t>
   </si>
@@ -425,6 +425,15 @@
   <si>
     <t>3. Search results returns with no matches message
 5. Search results returns with no matches message</t>
+  </si>
+  <si>
+    <t>1. Open https://abantecart.codifyme.co.nz
+2. I inspect Facebook link
+3. I inspect Twitter link</t>
+  </si>
+  <si>
+    <t>2. Link is correct and working (https://www.facebook.com/AbanteCart)
+3. Link is correct and working (https://twitter.com/abantecart)</t>
   </si>
 </sst>
 </file>
@@ -767,8 +776,8 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1102,21 +1111,27 @@
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>85</v>
       </c>
@@ -1129,8 +1144,14 @@
       <c r="D18" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E18" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>93</v>
       </c>
@@ -1144,7 +1165,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>86</v>
       </c>
@@ -1158,7 +1179,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="165" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>87</v>
       </c>
@@ -1172,7 +1193,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>88</v>
       </c>
@@ -1186,7 +1207,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>89</v>
       </c>
@@ -1197,7 +1218,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>90</v>
       </c>
@@ -1211,7 +1232,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>94</v>
       </c>

</xml_diff>

<commit_message>
Added 'Check Footer Social Media links are working' test script
</commit_message>
<xml_diff>
--- a/Test cases.xlsx
+++ b/Test cases.xlsx
@@ -777,7 +777,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,22 +1132,22 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E18" s="2" t="s">
+      <c r="D18" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="3" t="s">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added 'Check user can submit an enquiry using valid entries' test script
</commit_message>
<xml_diff>
--- a/Test cases.xlsx
+++ b/Test cases.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="107">
   <si>
     <t>ID</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>Expected Result</t>
-  </si>
-  <si>
-    <t>Status</t>
   </si>
   <si>
     <t>Remark</t>
@@ -145,9 +142,6 @@
     <t>Check all Homepage block elements are displayed</t>
   </si>
   <si>
-    <t>Check user can submit an enquiry</t>
-  </si>
-  <si>
     <t>Check all PLP block elements are displayed:
 • heading1
 • top sorting well
@@ -434,6 +428,41 @@
   <si>
     <t>2. Link is correct and working (https://www.facebook.com/AbanteCart)
 3. Link is correct and working (https://twitter.com/abantecart)</t>
+  </si>
+  <si>
+    <t>1. Open https://abantecart.codifyme.co.nz/
+2. Click Contact Us on the footer block
+3. Enter First name
+4. Enter Email
+5. Enter Enquiry message
+6. Click Submit</t>
+  </si>
+  <si>
+    <t>Test Data</t>
+  </si>
+  <si>
+    <t>7B</t>
+  </si>
+  <si>
+    <t>Check user cannot submit a blank enquiry</t>
+  </si>
+  <si>
+    <t>Check user can submit an enquiry using valid entries</t>
+  </si>
+  <si>
+    <t>1. Open https://abantecart.codifyme.co.nz/
+2. Click Contact Us on the footer block
+3. Leave all fields blank and click Submit</t>
+  </si>
+  <si>
+    <t>6. A message appears "Your enquiry has been successfully sent to the store owner!"
+https://abantecart.codifyme.co.nz/index.php?rt=content/contact/success</t>
+  </si>
+  <si>
+    <t>3. Each field returns with an error message:
+• First name: First name: is required field! Name must be between 3 and 32 characters!
+• Email: Email: is required field! E-Mail Address does not appear to be valid!
+• Enquiry: Enquiry: is required field! Enquiry must be between 10 and 3000 characters!</t>
   </si>
 </sst>
 </file>
@@ -773,11 +802,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,439 +840,465 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="3" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="3" customFormat="1" ht="240" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="2" t="s">
+      <c r="B22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="165" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="D22" s="2" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 'Check user cannot submit a blank enquiry' test script
</commit_message>
<xml_diff>
--- a/Test cases.xlsx
+++ b/Test cases.xlsx
@@ -450,19 +450,20 @@
     <t>Check user can submit an enquiry using valid entries</t>
   </si>
   <si>
+    <t>6. A message appears "Your enquiry has been successfully sent to the store owner!"
+https://abantecart.codifyme.co.nz/index.php?rt=content/contact/success</t>
+  </si>
+  <si>
     <t>1. Open https://abantecart.codifyme.co.nz/
 2. Click Contact Us on the footer block
-3. Leave all fields blank and click Submit</t>
-  </si>
-  <si>
-    <t>6. A message appears "Your enquiry has been successfully sent to the store owner!"
-https://abantecart.codifyme.co.nz/index.php?rt=content/contact/success</t>
+3. Leave all fields blank
+4. Click Submit</t>
   </si>
   <si>
     <t>3. Each field returns with an error message:
-• First name: First name: is required field! Name must be between 3 and 32 characters!
-• Email: Email: is required field! E-Mail Address does not appear to be valid!
-• Enquiry: Enquiry: is required field! Enquiry must be between 10 and 3000 characters!</t>
+• First name: is required field! Name must be between 3 and 32 characters!
+• Email: is required field! E-Mail Address does not appear to be valid!
+• Enquiry: is required field! Enquiry must be between 10 and 3000 characters!</t>
   </si>
 </sst>
 </file>
@@ -806,7 +807,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1197,26 +1198,26 @@
         <v>99</v>
       </c>
       <c r="F19" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="3" t="s">
         <v>106</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added 'Check Product List Page block or elements are displayed' test script
</commit_message>
<xml_diff>
--- a/Test cases.xlsx
+++ b/Test cases.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="109">
   <si>
     <t>ID</t>
   </si>
@@ -142,13 +142,6 @@
     <t>Check all Homepage block elements are displayed</t>
   </si>
   <si>
-    <t>Check all PLP block elements are displayed:
-• heading1
-• top sorting well
-• thumbnails grid
-• bottom sorting well</t>
-  </si>
-  <si>
     <t>Check all PDP block elements are displayed:
 • Latest products
 • thumbnails
@@ -464,6 +457,21 @@
 • First name: is required field! Name must be between 3 and 32 characters!
 • Email: is required field! E-Mail Address does not appear to be valid!
 • Enquiry: is required field! Enquiry must be between 10 and 3000 characters!</t>
+  </si>
+  <si>
+    <t>2. All element or blocks should be displayed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Product List Page block or elements are displayed
+</t>
+  </si>
+  <si>
+    <t>1. Open a Product List Page
+2. Inspect the following blocks:
+• Category header
+• Top sorting well
+• Product thumbnails
+• Bottom sorting well</t>
   </si>
 </sst>
 </file>
@@ -806,8 +814,8 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,7 +849,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -849,10 +857,10 @@
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>31</v>
@@ -861,29 +869,29 @@
         <v>29</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="3" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="3" customFormat="1" ht="240" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>8</v>
@@ -892,7 +900,7 @@
         <v>33</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>28</v>
@@ -903,7 +911,7 @@
     </row>
     <row r="5" spans="1:8" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>8</v>
@@ -912,38 +920,38 @@
         <v>7</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>9</v>
@@ -952,18 +960,18 @@
         <v>17</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>9</v>
@@ -972,18 +980,18 @@
         <v>18</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>9</v>
@@ -992,18 +1000,18 @@
         <v>19</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>9</v>
@@ -1012,18 +1020,18 @@
         <v>20</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>9</v>
@@ -1032,18 +1040,18 @@
         <v>21</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>9</v>
@@ -1052,18 +1060,18 @@
         <v>22</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>9</v>
@@ -1072,18 +1080,18 @@
         <v>23</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E13" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>9</v>
@@ -1092,58 +1100,58 @@
         <v>24</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E14" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E16" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>16</v>
@@ -1152,18 +1160,18 @@
         <v>25</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E17" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>16</v>
@@ -1172,92 +1180,98 @@
         <v>26</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E18" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E20" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="F20" s="3" t="s">
+    </row>
+    <row r="21" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>27</v>
@@ -1265,24 +1279,24 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>27</v>
@@ -1290,13 +1304,13 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>27</v>

</xml_diff>